<commit_message>
added rec func to find deep linkage
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -2094,9 +2094,10 @@
           <t>yoy growth</t>
         </is>
       </c>
-      <c r="C213">
-        <f>B195 / =B195 - 1</f>
-        <v/>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Total other income / Total other income - 1</t>
+        </is>
       </c>
     </row>
     <row r="214">
@@ -2105,9 +2106,10 @@
           <t>10 year CAGR</t>
         </is>
       </c>
-      <c r="C214">
-        <f>B195 / =B195 )^(1/10)-1</f>
-        <v/>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Total other income / Total other income )^(1/10)-1</t>
+        </is>
       </c>
     </row>
     <row r="215">
@@ -2116,9 +2118,10 @@
           <t>5 year CAGR</t>
         </is>
       </c>
-      <c r="C215">
-        <f>B195 / =B195 )^(1/5)-1</f>
-        <v/>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Total other income / Total other income )^(1/5)-1</t>
+        </is>
       </c>
     </row>
     <row r="216">
@@ -2127,9 +2130,10 @@
           <t>3 year CAGR</t>
         </is>
       </c>
-      <c r="C216">
-        <f>B195 / =B195 )^(1/3)-1</f>
-        <v/>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Total other income / Total other income )^(1/3)-1</t>
+        </is>
       </c>
     </row>
     <row r="219">
@@ -2461,7 +2465,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>FCFF / - =B249</t>
+          <t>FCFF / - Cash interest paid</t>
         </is>
       </c>
     </row>
@@ -2664,9 +2668,10 @@
           <t>yoy growth</t>
         </is>
       </c>
-      <c r="C305">
-        <f>B285 / =B285 - 1</f>
-        <v/>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Total tax / Total tax - 1</t>
+        </is>
       </c>
     </row>
     <row r="306">
@@ -2675,9 +2680,10 @@
           <t>10 year CAGR</t>
         </is>
       </c>
-      <c r="C306">
-        <f>B285 / =B285 )^(1/10)-1</f>
-        <v/>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Total tax / Total tax )^(1/10)-1</t>
+        </is>
       </c>
     </row>
     <row r="307">
@@ -2686,9 +2692,10 @@
           <t>5 year CAGR</t>
         </is>
       </c>
-      <c r="C307">
-        <f>B285 / =B285 )^(1/5)-1</f>
-        <v/>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Total tax / Total tax )^(1/5)-1</t>
+        </is>
       </c>
     </row>
     <row r="308">
@@ -2697,15 +2704,17 @@
           <t>3 year CAGR</t>
         </is>
       </c>
-      <c r="C308">
-        <f>B285 / =B285 )^(1/3)-1</f>
-        <v/>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Total tax / Total tax )^(1/3)-1</t>
+        </is>
       </c>
     </row>
     <row r="311">
-      <c r="C311">
-        <f>B285</f>
-        <v/>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Total tax</t>
+        </is>
       </c>
     </row>
     <row r="312">
@@ -2726,9 +2735,10 @@
           <t>Tax Rate</t>
         </is>
       </c>
-      <c r="C313">
-        <f>B299 / PBT</f>
-        <v/>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Total tax / PBT</t>
+        </is>
       </c>
     </row>
     <row r="316">
@@ -3739,9 +3749,10 @@
           <t>Ratio</t>
         </is>
       </c>
-      <c r="C450">
-        <f>B368 / Profit for controlling shareholders plus share of profit from associate and JV after preference dividend</f>
-        <v/>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>Retained profit / Profit for controlling shareholders plus share of profit from associate and JV after preference dividend</t>
+        </is>
       </c>
     </row>
     <row r="451">
@@ -3750,9 +3761,10 @@
           <t>yoy growth</t>
         </is>
       </c>
-      <c r="C451">
-        <f>B368 / =B368 - 1</f>
-        <v/>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>Retained profit / Retained profit - 1</t>
+        </is>
       </c>
     </row>
     <row r="453">
@@ -3979,7 +3991,7 @@
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>PBT Margin * (1- Effective Tax rate )* =B46 * Leverage</t>
+          <t>PBT Margin * (1- Effective Tax rate )* Total Asset turnover * Leverage</t>
         </is>
       </c>
     </row>
@@ -4034,9 +4046,10 @@
       </c>
     </row>
     <row r="487">
-      <c r="C487">
-        <f>B46</f>
-        <v/>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>Total Asset turnover</t>
+        </is>
       </c>
     </row>
     <row r="488">
@@ -4054,7 +4067,7 @@
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>EBIT Margin incl other income - Interest to Net Sales + Exceptional items to Net Sales )*(1- Effective Tax rate )* =B471 * =B472</t>
+          <t>EBIT Margin incl other income - Interest to Net Sales + Exceptional items to Net Sales )*(1- Effective Tax rate )* Total Asset turnover * Leverage</t>
         </is>
       </c>
     </row>
@@ -4710,7 +4723,7 @@
       </c>
       <c r="C596" t="inlineStr">
         <is>
-          <t>Dividend incl tax / =B367</t>
+          <t>Dividend incl tax / Profit for controlling shareholders plus share of profit from associate and JV after preference dividend</t>
         </is>
       </c>
     </row>
@@ -4741,7 +4754,7 @@
       </c>
       <c r="C601" t="inlineStr">
         <is>
-          <t>Dividend excl tax / =B365&amp;" after preference dividends"</t>
+          <t>Dividend excl tax / Consolidated PAT plus share of profit from associate and JV</t>
         </is>
       </c>
     </row>
@@ -4954,7 +4967,7 @@
       </c>
       <c r="C636" t="inlineStr">
         <is>
-          <t>Current maturity of Debentures &amp; Bonds + Current maturity - Others + Current maturity of Debentures &amp; Bonds + Current maturity - Others + SUM( Current maturity of Debentures &amp; Bonds : B193 )</t>
+          <t>Current maturity of Debentures &amp; Bonds + Current maturity - Others + Current maturity of Debentures &amp; Bonds + Current maturity - Others + SUM( Current maturity of Debentures &amp; Bonds : 193 )</t>
         </is>
       </c>
     </row>
@@ -5116,9 +5129,10 @@
           <t>Others</t>
         </is>
       </c>
-      <c r="C657">
-        <f>B$633 - SUM( Foreign Debt : Intercorporate deposits and loan from related party )</f>
-        <v/>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>Total Debt (LT and ST) - SUM( Foreign Debt : Intercorporate deposits and loan from related party )</t>
+        </is>
       </c>
     </row>
     <row r="659">
@@ -5953,14 +5967,15 @@
       </c>
       <c r="C792" t="inlineStr">
         <is>
-          <t>CWIP / =B759</t>
+          <t>CWIP / Total GB</t>
         </is>
       </c>
     </row>
     <row r="795">
-      <c r="C795">
-        <f>B759</f>
-        <v/>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>Total GB</t>
+        </is>
       </c>
     </row>
     <row r="796">
@@ -5978,7 +5993,7 @@
       </c>
       <c r="C797" t="inlineStr">
         <is>
-          <t>Accumulated Depreciation / =B763</t>
+          <t>Accumulated Depreciation / Total GB</t>
         </is>
       </c>
     </row>
@@ -6009,7 +6024,7 @@
       </c>
       <c r="C802" t="inlineStr">
         <is>
-          <t>Intangibles / =B372</t>
+          <t>Intangibles / Common Equity + Reserves</t>
         </is>
       </c>
     </row>
@@ -6021,9 +6036,10 @@
       </c>
     </row>
     <row r="806">
-      <c r="C806">
-        <f>B763</f>
-        <v/>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>Total GB</t>
+        </is>
       </c>
     </row>
     <row r="807">
@@ -6034,14 +6050,15 @@
       </c>
       <c r="C807" t="inlineStr">
         <is>
-          <t>Cash capex incl advances / =B790</t>
+          <t>Cash capex incl advances / Total GB</t>
         </is>
       </c>
     </row>
     <row r="810">
-      <c r="C810">
-        <f>B790</f>
-        <v/>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>Total GB</t>
+        </is>
       </c>
     </row>
     <row r="811">
@@ -6074,9 +6091,10 @@
           <t>Change in FA in BS</t>
         </is>
       </c>
-      <c r="C813">
-        <f>B795 : Capital Advances )-SUM( =B795 : Capital Advances )</f>
-        <v/>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>Total GB : Capital Advances )-SUM( Total GB : Capital Advances )</t>
+        </is>
       </c>
     </row>
     <row r="814">
@@ -6778,9 +6796,10 @@
           <t>Inventory days-average</t>
         </is>
       </c>
-      <c r="C925">
-        <f>'Ace-SBS'!A420 : ='Ace-SBS'!A420 )/ Net Sales</f>
-        <v/>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>Inventories : Inventories )/ Net Sales</t>
+        </is>
       </c>
     </row>
     <row r="926">
@@ -6789,9 +6808,10 @@
           <t>Inventory days-closing</t>
         </is>
       </c>
-      <c r="C926">
-        <f>'Ace-SBS'!A420 / Net Sales</f>
-        <v/>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>Inventories / Net Sales</t>
+        </is>
       </c>
     </row>
     <row r="928">
@@ -6814,9 +6834,10 @@
       </c>
     </row>
     <row r="930">
-      <c r="C930">
-        <f>'Ace-SBS'!A420</f>
-        <v/>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>Inventories</t>
+        </is>
       </c>
     </row>
     <row r="931">
@@ -6825,9 +6846,10 @@
           <t>Inventory days-average</t>
         </is>
       </c>
-      <c r="C931">
-        <f>B892 : =B892 )/ COGS</f>
-        <v/>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>Inventories : Inventories )/ COGS</t>
+        </is>
       </c>
     </row>
     <row r="932">
@@ -6836,9 +6858,10 @@
           <t>Inventory days-closing</t>
         </is>
       </c>
-      <c r="C932">
-        <f>B892 / COGS</f>
-        <v/>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>Inventories / COGS</t>
+        </is>
       </c>
     </row>
     <row r="934">
@@ -6868,9 +6891,10 @@
           <t>Debtor days-average</t>
         </is>
       </c>
-      <c r="C937">
-        <f>'Ace-SBS'!A433 : ='Ace-SBS'!A433 )/ Net Sales</f>
-        <v/>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>Sundry Debtors : Sundry Debtors )/ Net Sales</t>
+        </is>
       </c>
     </row>
     <row r="938">
@@ -6879,9 +6903,10 @@
           <t>Debtor days-closing</t>
         </is>
       </c>
-      <c r="C938">
-        <f>'Ace-SBS'!A433 / Net Sales</f>
-        <v/>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>Sundry Debtors / Net Sales</t>
+        </is>
       </c>
     </row>
     <row r="939">
@@ -7074,9 +7099,10 @@
           <t>Trade Payable days-average</t>
         </is>
       </c>
-      <c r="C966">
-        <f>'Ace-SBS'!A168 : ='Ace-SBS'!A168 )/ Net Sales</f>
-        <v/>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>Trade Payables : Trade Payables )/ Net Sales</t>
+        </is>
       </c>
     </row>
     <row r="967">
@@ -7085,9 +7111,10 @@
           <t>Trade Payable days-closing</t>
         </is>
       </c>
-      <c r="C967">
-        <f>'Ace-SBS'!A168 / Net Sales</f>
-        <v/>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>Trade Payables / Net Sales</t>
+        </is>
       </c>
     </row>
     <row r="969">
@@ -7105,9 +7132,10 @@
       </c>
     </row>
     <row r="971">
-      <c r="C971">
-        <f>'Ace-SBS'!A168</f>
-        <v/>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>Trade Payables</t>
+        </is>
       </c>
     </row>
     <row r="972">
@@ -7116,9 +7144,10 @@
           <t>Trade Payable days-average</t>
         </is>
       </c>
-      <c r="C972">
-        <f>B942 : =B942 )/ COGS</f>
-        <v/>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>Trade Payables : Trade Payables )/ COGS</t>
+        </is>
       </c>
     </row>
     <row r="973">
@@ -7127,9 +7156,10 @@
           <t>Trade Payable days-closing</t>
         </is>
       </c>
-      <c r="C973">
-        <f>B942 / COGS</f>
-        <v/>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>Trade Payables / COGS</t>
+        </is>
       </c>
     </row>
     <row r="976">
@@ -7460,7 +7490,7 @@
       </c>
       <c r="C1030" t="inlineStr">
         <is>
-          <t>Net Sales / ='Ace-SBS'!A23</t>
+          <t>Net Sales / Number of Equity Shares Paid Up</t>
         </is>
       </c>
     </row>
@@ -7498,7 +7528,7 @@
       </c>
       <c r="C1036" t="inlineStr">
         <is>
-          <t>Dividend excl tax / ='Ace-SBS'!A23</t>
+          <t>Dividend excl tax / Number of Equity Shares Paid Up</t>
         </is>
       </c>
     </row>
@@ -7536,7 +7566,7 @@
       </c>
       <c r="C1042" t="inlineStr">
         <is>
-          <t>Total Capital Employed ex cash and invt / ='Ace-SBS'!A23</t>
+          <t>Total Capital Employed ex cash and invt / Number of Equity Shares Paid Up</t>
         </is>
       </c>
     </row>
@@ -7574,7 +7604,7 @@
       </c>
       <c r="C1048" t="inlineStr">
         <is>
-          <t>Total Capital Employed / ='Ace-SBS'!A23</t>
+          <t>Total Capital Employed / Number of Equity Shares Paid Up</t>
         </is>
       </c>
     </row>
@@ -7612,7 +7642,7 @@
       </c>
       <c r="C1054" t="inlineStr">
         <is>
-          <t>Total Assets / ='Ace-SBS'!A23</t>
+          <t>Total Assets / Number of Equity Shares Paid Up</t>
         </is>
       </c>
     </row>
@@ -7650,7 +7680,7 @@
       </c>
       <c r="C1060" t="inlineStr">
         <is>
-          <t>CFO plus invt income less interest paid / ='Ace-SBS'!A23</t>
+          <t>CFO plus invt income less interest paid / Number of Equity Shares Paid Up</t>
         </is>
       </c>
     </row>
@@ -7688,7 +7718,7 @@
       </c>
       <c r="C1066" t="inlineStr">
         <is>
-          <t>FCFE / ='Ace-SBS'!A23</t>
+          <t>FCFE / Number of Equity Shares Paid Up</t>
         </is>
       </c>
     </row>
@@ -7712,9 +7742,10 @@
       </c>
     </row>
     <row r="1071">
-      <c r="C1071">
-        <f>'Ace-SBS'!A23</f>
-        <v/>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>Number of Equity Shares Paid Up</t>
+        </is>
       </c>
     </row>
     <row r="1072">
@@ -7723,9 +7754,10 @@
           <t>Capex per share</t>
         </is>
       </c>
-      <c r="C1072">
-        <f>B$187 / =B$1017</f>
-        <v/>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>Cash capex incl advances / Number of Equity Shares Paid Up</t>
+        </is>
       </c>
     </row>
     <row r="1073">
@@ -7820,7 +7852,7 @@
       </c>
       <c r="C1084" t="inlineStr">
         <is>
-          <t>FCFF + SUM( Increase / (Decrease) in Loan Funds : Ratio )+SUM( Interest Paid : C75 )+ Other Financial Activities</t>
+          <t>FCFF + SUM( Increase / (Decrease) in Loan Funds : Ratio )+SUM( Interest Paid : 75 )+ Other Financial Activities</t>
         </is>
       </c>
     </row>
@@ -8252,7 +8284,7 @@
       </c>
       <c r="C1149" t="inlineStr">
         <is>
-          <t>CFO after interest and preference dividends / - =B605</t>
+          <t>CFO after interest and preference dividends / - Dividends-equity</t>
         </is>
       </c>
     </row>
@@ -8442,7 +8474,7 @@
       </c>
       <c r="C1181" t="inlineStr">
         <is>
-          <t>CFO + =B605 )/ =B$634</t>
+          <t>CFO + Dividends-equity )/ Long term debt (incl Curr Mat)</t>
         </is>
       </c>
     </row>
@@ -8658,9 +8690,10 @@
           <t>Ratio</t>
         </is>
       </c>
-      <c r="C1221">
-        <f>B1021 / Year End Closing price</f>
-        <v/>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>Adjusted EPS / Year End Closing price</t>
+        </is>
       </c>
     </row>
     <row r="1224">
@@ -8728,7 +8761,7 @@
       </c>
       <c r="C1231" t="inlineStr">
         <is>
-          <t>Year End Closing price / ='Ace-SBS'!A518</t>
+          <t>Year End Closing price / Adjusted Book Value</t>
         </is>
       </c>
     </row>
@@ -8752,9 +8785,10 @@
           <t>Ratio</t>
         </is>
       </c>
-      <c r="C1236">
-        <f>B1214 / FCFE per share</f>
-        <v/>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>Year End Closing price / FCFE per share</t>
+        </is>
       </c>
     </row>
     <row r="1239">
@@ -8860,7 +8894,7 @@
       </c>
       <c r="C1253" t="inlineStr">
         <is>
-          <t>EV / =B358</t>
+          <t>EV / EBIT excl other income</t>
         </is>
       </c>
     </row>
@@ -8964,7 +8998,7 @@
       </c>
       <c r="C1273" t="inlineStr">
         <is>
-          <t>CFO plus investment income / =B$1244</t>
+          <t>CFO plus investment income / EV</t>
         </is>
       </c>
     </row>
@@ -8995,7 +9029,7 @@
       </c>
       <c r="C1278" t="inlineStr">
         <is>
-          <t>FCFF / =B$1244</t>
+          <t>FCFF / EV</t>
         </is>
       </c>
     </row>

</xml_diff>